<commit_message>
backup Tue Jun 30 15:56:10 PDT 2020
</commit_message>
<xml_diff>
--- a/data/raw/2020-05-18/sheet_all_tabs.xlsx
+++ b/data/raw/2020-05-18/sheet_all_tabs.xlsx
@@ -414,7 +414,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Hubei Province (China)</t>
+          <t>Hubei</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -764,7 +764,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Iran (Islamic Republic of)</t>
+          <t>Iran</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">

</xml_diff>